<commit_message>
pestañas de lectura de qr y reguistros
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -456,11 +456,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">SODA ½ LITRO * 12 </t>
+          <t xml:space="preserve">SODA 500CC * 12 PET </t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -469,11 +469,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SODA TALCA 2¼ LITRO PET* 6 U</t>
+          <t>SODA TALCA 2,25L PET* 6 U</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -482,11 +482,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">SIFÓN SODA TALCA 2 LT PET*6U </t>
+          <t xml:space="preserve">SIFON SODA TALCA 2 LT PET*6U </t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -495,11 +495,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TALCA COLA PET ½L DESC *12U</t>
+          <t xml:space="preserve">TALCA COLA PET 500CC DESC *12U </t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -508,11 +508,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">TALCA LIMA LIMON PT½L DSC*12U </t>
+          <t>TALCA LIMA LIMON PT 500CC DSC*12U</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -521,11 +521,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">TALCA NARANJA PT ½L DESC*12U </t>
+          <t xml:space="preserve">TALCA NARANJA PT 500CC DESC*12U </t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -534,11 +534,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">TALCA POMELO PET ½L DESC *12U </t>
+          <t xml:space="preserve">TALCA POMELO PET 500CC DESC *12U </t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -547,7 +547,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">TALCA COLA PET 2¼L DESC *6U </t>
+          <t xml:space="preserve">TALCA COLA PET 2,25L DESC *6U </t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -560,7 +560,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">TALCA LIMA LIMON PT2¼LDESC*6U </t>
+          <t xml:space="preserve">TALCA LIMA LIMON PT 2,25L DESC*6U </t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -573,7 +573,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">TALCA NARANJA PT 2¼L DESC *6U </t>
+          <t xml:space="preserve">TALCA NARANJA PT 2,25L DESC *6U </t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -586,7 +586,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">TALCA POMELO PT 2¼L DESC *6U </t>
+          <t xml:space="preserve">TALCA POMELO PT 2,25L DESC *6U </t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -612,7 +612,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TALCA LIMA LIMON PET 3L DESC*6 U</t>
+          <t xml:space="preserve">TALCA LIMA LIMON PET 3L DESC*6 U </t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -625,7 +625,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TALCA NARANJA 3L DESC *6U</t>
+          <t xml:space="preserve">TALCA NARANJA 3L DESC *6U </t>
         </is>
       </c>
       <c r="C15" t="n">

</xml_diff>